<commit_message>
Updated runs (new data files)
</commit_message>
<xml_diff>
--- a/Soil_data_Lorenzo_03_09_2024_enzymes.xlsx
+++ b/Soil_data_Lorenzo_03_09_2024_enzymes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20415"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BC3\HoliSoil\Lorenzo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leticia.perez\Desktop\Holi\Activation_energy\Activation_energy_LorenzoII\Activation_energy_HoliSoils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECFD7AD5-D4E6-43B4-AFE1-003E9B1C946F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C7F040C-390D-4ECF-AC03-3B9D7613C79F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1359,7 +1359,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1411,6 +1411,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1731,9 +1737,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AS281"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K270" sqref="K270"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A275" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U293" sqref="U293"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -17783,7 +17789,7 @@
       <c r="Q122" s="9"/>
       <c r="R122" s="9"/>
       <c r="S122" s="9"/>
-      <c r="T122" s="9">
+      <c r="T122" s="19">
         <v>0</v>
       </c>
       <c r="U122" s="9"/>
@@ -17906,7 +17912,7 @@
       <c r="Q123" s="9"/>
       <c r="R123" s="9"/>
       <c r="S123" s="9"/>
-      <c r="T123" s="9">
+      <c r="T123" s="19">
         <v>0</v>
       </c>
       <c r="U123" s="9"/>
@@ -18029,7 +18035,7 @@
       <c r="Q124" s="9"/>
       <c r="R124" s="9"/>
       <c r="S124" s="9"/>
-      <c r="T124" s="9">
+      <c r="T124" s="19">
         <v>0</v>
       </c>
       <c r="U124" s="9"/>
@@ -18152,7 +18158,7 @@
       <c r="Q125" s="9"/>
       <c r="R125" s="9"/>
       <c r="S125" s="9"/>
-      <c r="T125" s="9">
+      <c r="T125" s="19">
         <v>0</v>
       </c>
       <c r="U125" s="9"/>
@@ -18273,7 +18279,9 @@
       <c r="Q126" s="9"/>
       <c r="R126" s="9"/>
       <c r="S126" s="9"/>
-      <c r="T126" s="9"/>
+      <c r="T126" s="20">
+        <v>43.512499999999996</v>
+      </c>
       <c r="U126" s="9"/>
       <c r="V126" s="9"/>
       <c r="W126" s="9"/>
@@ -18392,7 +18400,9 @@
       <c r="Q127" s="9"/>
       <c r="R127" s="9"/>
       <c r="S127" s="9"/>
-      <c r="T127" s="9"/>
+      <c r="T127" s="20">
+        <v>43.512499999999996</v>
+      </c>
       <c r="U127" s="9"/>
       <c r="V127" s="9"/>
       <c r="W127" s="9"/>
@@ -18513,7 +18523,9 @@
       <c r="Q128" s="9"/>
       <c r="R128" s="9"/>
       <c r="S128" s="9"/>
-      <c r="T128" s="9"/>
+      <c r="T128" s="20">
+        <v>47.762499999999996</v>
+      </c>
       <c r="U128" s="9"/>
       <c r="V128" s="9"/>
       <c r="W128" s="9"/>
@@ -18634,7 +18646,9 @@
       <c r="Q129" s="9"/>
       <c r="R129" s="9"/>
       <c r="S129" s="9"/>
-      <c r="T129" s="9"/>
+      <c r="T129" s="20">
+        <v>47.762499999999996</v>
+      </c>
       <c r="U129" s="9"/>
       <c r="V129" s="9"/>
       <c r="W129" s="9"/>
@@ -18755,7 +18769,9 @@
       <c r="Q130" s="9"/>
       <c r="R130" s="9"/>
       <c r="S130" s="9"/>
-      <c r="T130" s="9"/>
+      <c r="T130" s="20">
+        <v>47.762499999999996</v>
+      </c>
       <c r="U130" s="9"/>
       <c r="V130" s="9"/>
       <c r="W130" s="9"/>
@@ -18876,7 +18892,9 @@
       <c r="Q131" s="9"/>
       <c r="R131" s="9"/>
       <c r="S131" s="9"/>
-      <c r="T131" s="9"/>
+      <c r="T131" s="20">
+        <v>47.762499999999996</v>
+      </c>
       <c r="U131" s="9"/>
       <c r="V131" s="9"/>
       <c r="W131" s="9"/>
@@ -18997,7 +19015,7 @@
       <c r="Q132" s="9"/>
       <c r="R132" s="9"/>
       <c r="S132" s="9"/>
-      <c r="T132" s="9">
+      <c r="T132" s="19">
         <v>0</v>
       </c>
       <c r="U132" s="9"/>
@@ -19120,7 +19138,7 @@
       <c r="Q133" s="9"/>
       <c r="R133" s="9"/>
       <c r="S133" s="9"/>
-      <c r="T133" s="9">
+      <c r="T133" s="19">
         <v>0</v>
       </c>
       <c r="U133" s="9"/>
@@ -19243,7 +19261,7 @@
       <c r="Q134" s="9"/>
       <c r="R134" s="9"/>
       <c r="S134" s="9"/>
-      <c r="T134" s="9">
+      <c r="T134" s="19">
         <v>0</v>
       </c>
       <c r="U134" s="9"/>
@@ -19366,7 +19384,7 @@
       <c r="Q135" s="9"/>
       <c r="R135" s="9"/>
       <c r="S135" s="9"/>
-      <c r="T135" s="9">
+      <c r="T135" s="19">
         <v>0</v>
       </c>
       <c r="U135" s="9"/>
@@ -19489,7 +19507,9 @@
       <c r="Q136" s="9"/>
       <c r="R136" s="9"/>
       <c r="S136" s="9"/>
-      <c r="T136" s="9"/>
+      <c r="T136" s="20">
+        <v>55.75</v>
+      </c>
       <c r="U136" s="9"/>
       <c r="V136" s="9"/>
       <c r="W136" s="9"/>
@@ -19610,7 +19630,9 @@
       <c r="Q137" s="9"/>
       <c r="R137" s="9"/>
       <c r="S137" s="9"/>
-      <c r="T137" s="9"/>
+      <c r="T137" s="20">
+        <v>55.75</v>
+      </c>
       <c r="U137" s="9"/>
       <c r="V137" s="9"/>
       <c r="W137" s="9"/>
@@ -19731,7 +19753,9 @@
       <c r="Q138" s="9"/>
       <c r="R138" s="9"/>
       <c r="S138" s="9"/>
-      <c r="T138" s="9"/>
+      <c r="T138" s="20">
+        <v>55.75</v>
+      </c>
       <c r="U138" s="9"/>
       <c r="V138" s="9"/>
       <c r="W138" s="9"/>
@@ -19852,7 +19876,9 @@
       <c r="Q139" s="9"/>
       <c r="R139" s="9"/>
       <c r="S139" s="9"/>
-      <c r="T139" s="9"/>
+      <c r="T139" s="20">
+        <v>55.75</v>
+      </c>
       <c r="U139" s="9"/>
       <c r="V139" s="9"/>
       <c r="W139" s="9"/>
@@ -19971,7 +19997,9 @@
       <c r="Q140" s="9"/>
       <c r="R140" s="9"/>
       <c r="S140" s="9"/>
-      <c r="T140" s="9"/>
+      <c r="T140" s="20">
+        <v>48.859999999999992</v>
+      </c>
       <c r="U140" s="9"/>
       <c r="V140" s="9"/>
       <c r="W140" s="9"/>
@@ -20090,7 +20118,9 @@
       <c r="Q141" s="9"/>
       <c r="R141" s="9"/>
       <c r="S141" s="9"/>
-      <c r="T141" s="9"/>
+      <c r="T141" s="20">
+        <v>48.859999999999992</v>
+      </c>
       <c r="U141" s="9"/>
       <c r="V141" s="9"/>
       <c r="W141" s="9"/>
@@ -20211,7 +20241,7 @@
       <c r="Q142" s="9"/>
       <c r="R142" s="9"/>
       <c r="S142" s="9"/>
-      <c r="T142" s="9">
+      <c r="T142" s="19">
         <v>0</v>
       </c>
       <c r="U142" s="9"/>
@@ -20334,7 +20364,7 @@
       <c r="Q143" s="9"/>
       <c r="R143" s="9"/>
       <c r="S143" s="9"/>
-      <c r="T143" s="9">
+      <c r="T143" s="19">
         <v>0</v>
       </c>
       <c r="U143" s="9"/>
@@ -20457,7 +20487,7 @@
       <c r="Q144" s="9"/>
       <c r="R144" s="9"/>
       <c r="S144" s="9"/>
-      <c r="T144" s="9">
+      <c r="T144" s="19">
         <v>0</v>
       </c>
       <c r="U144" s="9"/>
@@ -20580,7 +20610,7 @@
       <c r="Q145" s="9"/>
       <c r="R145" s="9"/>
       <c r="S145" s="9"/>
-      <c r="T145" s="9">
+      <c r="T145" s="19">
         <v>0</v>
       </c>
       <c r="U145" s="9"/>
@@ -20701,7 +20731,9 @@
       <c r="Q146" s="9"/>
       <c r="R146" s="9"/>
       <c r="S146" s="9"/>
-      <c r="T146" s="9"/>
+      <c r="T146" s="20">
+        <v>43.169230769230772</v>
+      </c>
       <c r="U146" s="9"/>
       <c r="V146" s="9"/>
       <c r="W146" s="9"/>
@@ -20820,7 +20852,9 @@
       <c r="Q147" s="9"/>
       <c r="R147" s="9"/>
       <c r="S147" s="9"/>
-      <c r="T147" s="9"/>
+      <c r="T147" s="20">
+        <v>43.169230769230772</v>
+      </c>
       <c r="U147" s="9"/>
       <c r="V147" s="9"/>
       <c r="W147" s="9"/>
@@ -20941,7 +20975,9 @@
       <c r="Q148" s="9"/>
       <c r="R148" s="9"/>
       <c r="S148" s="9"/>
-      <c r="T148" s="9"/>
+      <c r="T148" s="20">
+        <v>51.127272727272725</v>
+      </c>
       <c r="U148" s="9"/>
       <c r="V148" s="9"/>
       <c r="W148" s="9"/>
@@ -21062,7 +21098,9 @@
       <c r="Q149" s="9"/>
       <c r="R149" s="9"/>
       <c r="S149" s="9"/>
-      <c r="T149" s="9"/>
+      <c r="T149" s="20">
+        <v>51.127272727272725</v>
+      </c>
       <c r="U149" s="9"/>
       <c r="V149" s="9"/>
       <c r="W149" s="9"/>
@@ -21183,7 +21221,9 @@
       <c r="Q150" s="9"/>
       <c r="R150" s="9"/>
       <c r="S150" s="9"/>
-      <c r="T150" s="9"/>
+      <c r="T150" s="20">
+        <v>51.127272727272725</v>
+      </c>
       <c r="U150" s="9"/>
       <c r="V150" s="9"/>
       <c r="W150" s="9"/>
@@ -21304,7 +21344,9 @@
       <c r="Q151" s="9"/>
       <c r="R151" s="9"/>
       <c r="S151" s="9"/>
-      <c r="T151" s="9"/>
+      <c r="T151" s="20">
+        <v>51.127272727272725</v>
+      </c>
       <c r="U151" s="9"/>
       <c r="V151" s="9"/>
       <c r="W151" s="9"/>
@@ -21425,7 +21467,7 @@
       <c r="Q152" s="9"/>
       <c r="R152" s="9"/>
       <c r="S152" s="9"/>
-      <c r="T152" s="9">
+      <c r="T152" s="19">
         <v>0</v>
       </c>
       <c r="U152" s="9"/>
@@ -21548,7 +21590,7 @@
       <c r="Q153" s="9"/>
       <c r="R153" s="9"/>
       <c r="S153" s="9"/>
-      <c r="T153" s="9">
+      <c r="T153" s="19">
         <v>0</v>
       </c>
       <c r="U153" s="9"/>
@@ -21671,7 +21713,7 @@
       <c r="Q154" s="9"/>
       <c r="R154" s="9"/>
       <c r="S154" s="9"/>
-      <c r="T154" s="9">
+      <c r="T154" s="19">
         <v>0</v>
       </c>
       <c r="U154" s="9"/>
@@ -21794,7 +21836,7 @@
       <c r="Q155" s="9"/>
       <c r="R155" s="9"/>
       <c r="S155" s="9"/>
-      <c r="T155" s="9">
+      <c r="T155" s="19">
         <v>0</v>
       </c>
       <c r="U155" s="9"/>
@@ -21917,7 +21959,9 @@
       <c r="Q156" s="9"/>
       <c r="R156" s="9"/>
       <c r="S156" s="9"/>
-      <c r="T156" s="9"/>
+      <c r="T156" s="20">
+        <v>54.616666666666667</v>
+      </c>
       <c r="U156" s="9"/>
       <c r="V156" s="9"/>
       <c r="W156" s="9"/>
@@ -22038,7 +22082,9 @@
       <c r="Q157" s="9"/>
       <c r="R157" s="9"/>
       <c r="S157" s="9"/>
-      <c r="T157" s="9"/>
+      <c r="T157" s="20">
+        <v>54.616666666666667</v>
+      </c>
       <c r="U157" s="9"/>
       <c r="V157" s="9"/>
       <c r="W157" s="9"/>
@@ -22159,7 +22205,9 @@
       <c r="Q158" s="9"/>
       <c r="R158" s="9"/>
       <c r="S158" s="9"/>
-      <c r="T158" s="9"/>
+      <c r="T158" s="20">
+        <v>54.616666666666667</v>
+      </c>
       <c r="U158" s="9"/>
       <c r="V158" s="9"/>
       <c r="W158" s="9"/>
@@ -22280,7 +22328,9 @@
       <c r="Q159" s="9"/>
       <c r="R159" s="9"/>
       <c r="S159" s="9"/>
-      <c r="T159" s="9"/>
+      <c r="T159" s="20">
+        <v>54.616666666666667</v>
+      </c>
       <c r="U159" s="9"/>
       <c r="V159" s="9"/>
       <c r="W159" s="9"/>
@@ -22399,7 +22449,9 @@
       <c r="Q160" s="9"/>
       <c r="R160" s="9"/>
       <c r="S160" s="9"/>
-      <c r="T160" s="9"/>
+      <c r="T160" s="20">
+        <v>47.667391304347831</v>
+      </c>
       <c r="U160" s="9"/>
       <c r="V160" s="9"/>
       <c r="W160" s="9"/>
@@ -22518,7 +22570,9 @@
       <c r="Q161" s="9"/>
       <c r="R161" s="9"/>
       <c r="S161" s="9"/>
-      <c r="T161" s="9"/>
+      <c r="T161" s="20">
+        <v>47.667391304347831</v>
+      </c>
       <c r="U161" s="9"/>
       <c r="V161" s="9"/>
       <c r="W161" s="9"/>
@@ -22639,7 +22693,7 @@
       <c r="Q162" s="9"/>
       <c r="R162" s="9"/>
       <c r="S162" s="9"/>
-      <c r="T162" s="9">
+      <c r="T162" s="19">
         <v>0</v>
       </c>
       <c r="U162" s="9"/>
@@ -22760,7 +22814,7 @@
       <c r="Q163" s="9"/>
       <c r="R163" s="9"/>
       <c r="S163" s="9"/>
-      <c r="T163" s="9">
+      <c r="T163" s="19">
         <v>0</v>
       </c>
       <c r="U163" s="9"/>
@@ -22881,7 +22935,7 @@
       <c r="Q164" s="9"/>
       <c r="R164" s="9"/>
       <c r="S164" s="9"/>
-      <c r="T164" s="9">
+      <c r="T164" s="19">
         <v>0</v>
       </c>
       <c r="U164" s="9"/>
@@ -23002,7 +23056,7 @@
       <c r="Q165" s="9"/>
       <c r="R165" s="9"/>
       <c r="S165" s="9"/>
-      <c r="T165" s="9">
+      <c r="T165" s="19">
         <v>0</v>
       </c>
       <c r="U165" s="9"/>
@@ -23121,7 +23175,9 @@
       <c r="Q166" s="9"/>
       <c r="R166" s="9"/>
       <c r="S166" s="9"/>
-      <c r="T166" s="9"/>
+      <c r="T166" s="20">
+        <v>43.512499999999996</v>
+      </c>
       <c r="U166" s="9"/>
       <c r="V166" s="9"/>
       <c r="W166" s="9"/>
@@ -23238,7 +23294,9 @@
       <c r="Q167" s="9"/>
       <c r="R167" s="9"/>
       <c r="S167" s="9"/>
-      <c r="T167" s="9"/>
+      <c r="T167" s="20">
+        <v>43.512499999999996</v>
+      </c>
       <c r="U167" s="9"/>
       <c r="V167" s="9"/>
       <c r="W167" s="9"/>
@@ -23357,7 +23415,9 @@
       <c r="Q168" s="9"/>
       <c r="R168" s="9"/>
       <c r="S168" s="9"/>
-      <c r="T168" s="9"/>
+      <c r="T168" s="20">
+        <v>47.762499999999996</v>
+      </c>
       <c r="U168" s="9"/>
       <c r="V168" s="9"/>
       <c r="W168" s="9"/>
@@ -23476,7 +23536,9 @@
       <c r="Q169" s="9"/>
       <c r="R169" s="9"/>
       <c r="S169" s="9"/>
-      <c r="T169" s="9"/>
+      <c r="T169" s="20">
+        <v>47.762499999999996</v>
+      </c>
       <c r="U169" s="9"/>
       <c r="V169" s="9"/>
       <c r="W169" s="9"/>
@@ -23595,7 +23657,9 @@
       <c r="Q170" s="9"/>
       <c r="R170" s="9"/>
       <c r="S170" s="9"/>
-      <c r="T170" s="9"/>
+      <c r="T170" s="20">
+        <v>47.762499999999996</v>
+      </c>
       <c r="U170" s="9"/>
       <c r="V170" s="9"/>
       <c r="W170" s="9"/>
@@ -23714,7 +23778,9 @@
       <c r="Q171" s="9"/>
       <c r="R171" s="9"/>
       <c r="S171" s="9"/>
-      <c r="T171" s="9"/>
+      <c r="T171" s="20">
+        <v>47.762499999999996</v>
+      </c>
       <c r="U171" s="9"/>
       <c r="V171" s="9"/>
       <c r="W171" s="9"/>
@@ -23833,7 +23899,7 @@
       <c r="Q172" s="9"/>
       <c r="R172" s="9"/>
       <c r="S172" s="9"/>
-      <c r="T172" s="9">
+      <c r="T172" s="19">
         <v>0</v>
       </c>
       <c r="U172" s="9"/>
@@ -23954,7 +24020,7 @@
       <c r="Q173" s="9"/>
       <c r="R173" s="9"/>
       <c r="S173" s="9"/>
-      <c r="T173" s="9">
+      <c r="T173" s="19">
         <v>0</v>
       </c>
       <c r="U173" s="9"/>
@@ -24075,7 +24141,7 @@
       <c r="Q174" s="9"/>
       <c r="R174" s="9"/>
       <c r="S174" s="9"/>
-      <c r="T174" s="9">
+      <c r="T174" s="19">
         <v>0</v>
       </c>
       <c r="U174" s="9"/>
@@ -24196,7 +24262,7 @@
       <c r="Q175" s="9"/>
       <c r="R175" s="9"/>
       <c r="S175" s="9"/>
-      <c r="T175" s="9">
+      <c r="T175" s="19">
         <v>0</v>
       </c>
       <c r="U175" s="9"/>
@@ -24317,7 +24383,9 @@
       <c r="Q176" s="9"/>
       <c r="R176" s="9"/>
       <c r="S176" s="9"/>
-      <c r="T176" s="9"/>
+      <c r="T176" s="20">
+        <v>55.75</v>
+      </c>
       <c r="U176" s="9"/>
       <c r="V176" s="9"/>
       <c r="W176" s="9"/>
@@ -24436,7 +24504,9 @@
       <c r="Q177" s="9"/>
       <c r="R177" s="9"/>
       <c r="S177" s="9"/>
-      <c r="T177" s="9"/>
+      <c r="T177" s="20">
+        <v>55.75</v>
+      </c>
       <c r="U177" s="9"/>
       <c r="V177" s="9"/>
       <c r="W177" s="9"/>
@@ -24555,7 +24625,9 @@
       <c r="Q178" s="9"/>
       <c r="R178" s="9"/>
       <c r="S178" s="9"/>
-      <c r="T178" s="9"/>
+      <c r="T178" s="20">
+        <v>55.75</v>
+      </c>
       <c r="U178" s="9"/>
       <c r="V178" s="9"/>
       <c r="W178" s="9"/>
@@ -24674,7 +24746,9 @@
       <c r="Q179" s="9"/>
       <c r="R179" s="9"/>
       <c r="S179" s="9"/>
-      <c r="T179" s="9"/>
+      <c r="T179" s="20">
+        <v>55.75</v>
+      </c>
       <c r="U179" s="9"/>
       <c r="V179" s="9"/>
       <c r="W179" s="9"/>
@@ -24791,7 +24865,9 @@
       <c r="Q180" s="9"/>
       <c r="R180" s="9"/>
       <c r="S180" s="9"/>
-      <c r="T180" s="9"/>
+      <c r="T180" s="20">
+        <v>48.859999999999992</v>
+      </c>
       <c r="U180" s="9"/>
       <c r="V180" s="9"/>
       <c r="W180" s="9"/>
@@ -24908,7 +24984,9 @@
       <c r="Q181" s="9"/>
       <c r="R181" s="9"/>
       <c r="S181" s="9"/>
-      <c r="T181" s="9"/>
+      <c r="T181" s="20">
+        <v>48.859999999999992</v>
+      </c>
       <c r="U181" s="9"/>
       <c r="V181" s="9"/>
       <c r="W181" s="9"/>
@@ -25027,7 +25105,7 @@
       <c r="Q182" s="9"/>
       <c r="R182" s="9"/>
       <c r="S182" s="9"/>
-      <c r="T182" s="9">
+      <c r="T182" s="19">
         <v>0</v>
       </c>
       <c r="U182" s="9"/>
@@ -25148,7 +25226,7 @@
       <c r="Q183" s="9"/>
       <c r="R183" s="9"/>
       <c r="S183" s="9"/>
-      <c r="T183" s="9">
+      <c r="T183" s="19">
         <v>0</v>
       </c>
       <c r="U183" s="9"/>
@@ -25269,7 +25347,7 @@
       <c r="Q184" s="9"/>
       <c r="R184" s="9"/>
       <c r="S184" s="9"/>
-      <c r="T184" s="9">
+      <c r="T184" s="19">
         <v>0</v>
       </c>
       <c r="U184" s="9"/>
@@ -25390,7 +25468,7 @@
       <c r="Q185" s="9"/>
       <c r="R185" s="9"/>
       <c r="S185" s="9"/>
-      <c r="T185" s="9">
+      <c r="T185" s="19">
         <v>0</v>
       </c>
       <c r="U185" s="9"/>
@@ -25509,7 +25587,9 @@
       <c r="Q186" s="9"/>
       <c r="R186" s="9"/>
       <c r="S186" s="9"/>
-      <c r="T186" s="9"/>
+      <c r="T186" s="20">
+        <v>43.169230769230772</v>
+      </c>
       <c r="U186" s="9"/>
       <c r="V186" s="9"/>
       <c r="W186" s="9"/>
@@ -25626,7 +25706,9 @@
       <c r="Q187" s="9"/>
       <c r="R187" s="9"/>
       <c r="S187" s="9"/>
-      <c r="T187" s="9"/>
+      <c r="T187" s="20">
+        <v>43.169230769230772</v>
+      </c>
       <c r="U187" s="9"/>
       <c r="V187" s="9"/>
       <c r="W187" s="9"/>
@@ -25745,7 +25827,9 @@
       <c r="Q188" s="9"/>
       <c r="R188" s="9"/>
       <c r="S188" s="9"/>
-      <c r="T188" s="9"/>
+      <c r="T188" s="20">
+        <v>51.127272727272725</v>
+      </c>
       <c r="U188" s="9"/>
       <c r="V188" s="9"/>
       <c r="W188" s="9"/>
@@ -25864,7 +25948,9 @@
       <c r="Q189" s="9"/>
       <c r="R189" s="9"/>
       <c r="S189" s="9"/>
-      <c r="T189" s="9"/>
+      <c r="T189" s="20">
+        <v>51.127272727272725</v>
+      </c>
       <c r="U189" s="9"/>
       <c r="V189" s="9"/>
       <c r="W189" s="9"/>
@@ -25983,7 +26069,9 @@
       <c r="Q190" s="9"/>
       <c r="R190" s="9"/>
       <c r="S190" s="9"/>
-      <c r="T190" s="9"/>
+      <c r="T190" s="20">
+        <v>51.127272727272725</v>
+      </c>
       <c r="U190" s="9"/>
       <c r="V190" s="9"/>
       <c r="W190" s="9"/>
@@ -26102,7 +26190,9 @@
       <c r="Q191" s="9"/>
       <c r="R191" s="9"/>
       <c r="S191" s="9"/>
-      <c r="T191" s="9"/>
+      <c r="T191" s="20">
+        <v>51.127272727272725</v>
+      </c>
       <c r="U191" s="9"/>
       <c r="V191" s="9"/>
       <c r="W191" s="9"/>
@@ -26221,7 +26311,7 @@
       <c r="Q192" s="9"/>
       <c r="R192" s="9"/>
       <c r="S192" s="9"/>
-      <c r="T192" s="9">
+      <c r="T192" s="19">
         <v>0</v>
       </c>
       <c r="U192" s="9"/>
@@ -26342,7 +26432,7 @@
       <c r="Q193" s="9"/>
       <c r="R193" s="9"/>
       <c r="S193" s="9"/>
-      <c r="T193" s="9">
+      <c r="T193" s="19">
         <v>0</v>
       </c>
       <c r="U193" s="9"/>
@@ -26463,7 +26553,7 @@
       <c r="Q194" s="9"/>
       <c r="R194" s="9"/>
       <c r="S194" s="9"/>
-      <c r="T194" s="9">
+      <c r="T194" s="19">
         <v>0</v>
       </c>
       <c r="U194" s="9"/>
@@ -26584,7 +26674,7 @@
       <c r="Q195" s="9"/>
       <c r="R195" s="9"/>
       <c r="S195" s="9"/>
-      <c r="T195" s="9">
+      <c r="T195" s="19">
         <v>0</v>
       </c>
       <c r="U195" s="9"/>
@@ -26705,7 +26795,9 @@
       <c r="Q196" s="9"/>
       <c r="R196" s="9"/>
       <c r="S196" s="9"/>
-      <c r="T196" s="9"/>
+      <c r="T196" s="20">
+        <v>54.616666666666667</v>
+      </c>
       <c r="U196" s="9"/>
       <c r="V196" s="9"/>
       <c r="W196" s="9"/>
@@ -26824,7 +26916,9 @@
       <c r="Q197" s="9"/>
       <c r="R197" s="9"/>
       <c r="S197" s="9"/>
-      <c r="T197" s="9"/>
+      <c r="T197" s="20">
+        <v>54.616666666666667</v>
+      </c>
       <c r="U197" s="9"/>
       <c r="V197" s="9"/>
       <c r="W197" s="9"/>
@@ -26943,7 +27037,9 @@
       <c r="Q198" s="9"/>
       <c r="R198" s="9"/>
       <c r="S198" s="9"/>
-      <c r="T198" s="9"/>
+      <c r="T198" s="20">
+        <v>54.616666666666667</v>
+      </c>
       <c r="U198" s="9"/>
       <c r="V198" s="9"/>
       <c r="W198" s="9"/>
@@ -27062,7 +27158,9 @@
       <c r="Q199" s="9"/>
       <c r="R199" s="9"/>
       <c r="S199" s="9"/>
-      <c r="T199" s="9"/>
+      <c r="T199" s="20">
+        <v>54.616666666666667</v>
+      </c>
       <c r="U199" s="9"/>
       <c r="V199" s="9"/>
       <c r="W199" s="9"/>
@@ -27179,7 +27277,9 @@
       <c r="Q200" s="9"/>
       <c r="R200" s="9"/>
       <c r="S200" s="9"/>
-      <c r="T200" s="9"/>
+      <c r="T200" s="20">
+        <v>47.667391304347831</v>
+      </c>
       <c r="U200" s="9"/>
       <c r="V200" s="9"/>
       <c r="W200" s="9"/>
@@ -27296,7 +27396,9 @@
       <c r="Q201" s="9"/>
       <c r="R201" s="9"/>
       <c r="S201" s="9"/>
-      <c r="T201" s="9"/>
+      <c r="T201" s="20">
+        <v>47.667391304347831</v>
+      </c>
       <c r="U201" s="9"/>
       <c r="V201" s="9"/>
       <c r="W201" s="9"/>

</xml_diff>